<commit_message>
Added screenshots and reporting
</commit_message>
<xml_diff>
--- a/TestCases/UAT/UAT_Sanity_Suite.xlsx
+++ b/TestCases/UAT/UAT_Sanity_Suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\OrangeHRMLive\TestCases\UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C952CDB0-3709-4F17-8A9C-A61F368D37A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E28E4C-670E-4923-A92D-5C50FAC63F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="62">
   <si>
     <t>TestCase_Id</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Login with blank username</t>
   </si>
   <si>
-    <t>Login with blank password</t>
-  </si>
-  <si>
     <t>Login with invalid credentions</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>Click on login button</t>
   </si>
   <si>
-    <t>TC_006</t>
-  </si>
-  <si>
     <t>Navigate to URL and verify UI</t>
   </si>
   <si>
@@ -188,6 +182,36 @@
   </si>
   <si>
     <t>LOGIN_LOGIN_BUTTON</t>
+  </si>
+  <si>
+    <t>Enter password</t>
+  </si>
+  <si>
+    <t>qwerty</t>
+  </si>
+  <si>
+    <t>Enter invalid username</t>
+  </si>
+  <si>
+    <t>Enter invalid password</t>
+  </si>
+  <si>
+    <t>qweq</t>
+  </si>
+  <si>
+    <t>qeqe</t>
+  </si>
+  <si>
+    <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>Verify invalid credentials validation message</t>
+  </si>
+  <si>
+    <t>LOGIN_INVALID_CREDENTIALS_ERROR_LABEL</t>
+  </si>
+  <si>
+    <t>BLANK</t>
   </si>
 </sst>
 </file>
@@ -560,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,10 +622,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="1"/>
@@ -615,7 +639,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="1"/>
@@ -629,7 +653,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="1"/>
@@ -643,7 +667,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="1"/>
@@ -657,25 +681,11 @@
         <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -686,10 +696,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11624E8-9288-4831-9E39-FE5F7FB8109E}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -708,25 +718,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -734,17 +744,17 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -754,16 +764,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -774,17 +784,17 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -794,18 +804,20 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
@@ -814,18 +826,20 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
@@ -834,16 +848,16 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -854,19 +868,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -876,62 +890,194 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
fenkins file update 1
</commit_message>
<xml_diff>
--- a/TestCases/UAT/UAT_Sanity_Suite.xlsx
+++ b/TestCases/UAT/UAT_Sanity_Suite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\OrangeHRMLive\TestCases\UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E28E4C-670E-4923-A92D-5C50FAC63F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78379B5-9AD8-4471-A636-A81B1FCE11A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="92">
   <si>
     <t>TestCase_Id</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>TestStep_Id</t>
   </si>
   <si>
@@ -212,6 +209,99 @@
   </si>
   <si>
     <t>BLANK</t>
+  </si>
+  <si>
+    <t>Enter valid username</t>
+  </si>
+  <si>
+    <t>Enter valid password</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>TC_006</t>
+  </si>
+  <si>
+    <t>Log out</t>
+  </si>
+  <si>
+    <t>Click on user profile</t>
+  </si>
+  <si>
+    <t>HOME_ORANGE_HRM_USER_PROFILE</t>
+  </si>
+  <si>
+    <t>Login is successful</t>
+  </si>
+  <si>
+    <t>HOME_ORANGE_HRM_LOGO,HOME_ORANGE_HRM_USER_PROFILE</t>
+  </si>
+  <si>
+    <t>HOME_LOGOUT</t>
+  </si>
+  <si>
+    <t>Click on logout link</t>
+  </si>
+  <si>
+    <t>Verify logout is success</t>
+  </si>
+  <si>
+    <t>TC_007</t>
+  </si>
+  <si>
+    <t>Add a Employee from PIM menu</t>
+  </si>
+  <si>
+    <t>Click on PIM in menu bar</t>
+  </si>
+  <si>
+    <t>HOME_MENUBAR_PIM</t>
+  </si>
+  <si>
+    <t>PIM_ADD_EMPLOYEE_BUTTON</t>
+  </si>
+  <si>
+    <t>Click on Add employee button in PIM</t>
+  </si>
+  <si>
+    <t>PIM_ADD_EMPLOYEE_FIRST_NAME_TEXT_FIELD</t>
+  </si>
+  <si>
+    <t>PIM_ADD_EMPLOYEE_MIDDLE_NAME_TEXT_FIELD</t>
+  </si>
+  <si>
+    <t>PIM_ADD_EMPLOYEE_LAST_NAME_TEXT_FIELD</t>
+  </si>
+  <si>
+    <t>PIM_ADD_EMPLOYEE_SAVE_BUTTON</t>
+  </si>
+  <si>
+    <t>Enter employee first name</t>
+  </si>
+  <si>
+    <t>Enter employee middle name</t>
+  </si>
+  <si>
+    <t>Enter employee last name</t>
+  </si>
+  <si>
+    <t>Click on Save amployee button</t>
+  </si>
+  <si>
+    <t>TS_006</t>
+  </si>
+  <si>
+    <t>Snehal</t>
+  </si>
+  <si>
+    <t>Minal</t>
+  </si>
+  <si>
+    <t>Kumal</t>
   </si>
 </sst>
 </file>
@@ -249,7 +339,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -285,11 +375,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -302,6 +403,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -584,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,7 +729,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>15</v>
@@ -681,11 +788,39 @@
         <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -696,10 +831,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11624E8-9288-4831-9E39-FE5F7FB8109E}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,25 +853,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -744,17 +879,17 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -764,16 +899,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -784,17 +919,17 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -804,19 +939,19 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -826,19 +961,19 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -848,16 +983,16 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -868,19 +1003,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -890,19 +1025,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -912,19 +1047,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -934,19 +1069,19 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -956,16 +1091,16 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -976,19 +1111,19 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -998,19 +1133,19 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1020,19 +1155,19 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1042,16 +1177,16 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1062,22 +1197,262 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>